<commit_message>
some changes in dz_1
</commit_message>
<xml_diff>
--- a/dz_1.xlsx
+++ b/dz_1.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>1. зареєструватися на гіті</t>
   </si>
@@ -219,6 +219,43 @@
   </si>
   <si>
     <t>в текстовом файле, в верхней строке написать коментарий к Коммиту</t>
+  </si>
+  <si>
+    <t>git commit -m 'тест комментария к Коммиту'</t>
+  </si>
+  <si>
+    <t>это если без блокнота</t>
+  </si>
+  <si>
+    <t>https://ohshitgit.com/ru</t>
+  </si>
+  <si>
+    <t>10 полезных команд Git</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git log  (git log --graph)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - история всех изменений в ветке</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -323,7 +360,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,6 +393,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -651,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -665,6 +703,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
+      <c r="A1" s="14" t="s">
+        <v>31</v>
+      </c>
       <c r="B1" s="11" t="s">
         <v>21</v>
       </c>
@@ -792,48 +833,72 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" ht="31.8">
-      <c r="A18" s="3" t="s">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" ht="31.8">
+      <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B20" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="G13" r:id="rId2"/>
+    <hyperlink ref="A1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>